<commit_message>
adiciona tls e sasl
</commit_message>
<xml_diff>
--- a/MapeamentoModelovsRFC.xlsx
+++ b/MapeamentoModelovsRFC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\Mestrado\Estudo Orientado I\Formalização XMPP\1. Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E38AC087-5FA5-40CA-A393-D69EB34164B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F35BE3-AF14-4250-ADF1-3A4084CBFECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{3EC95438-80F5-49CB-918F-D44E3AA27D60}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$E$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$E$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -499,7 +499,7 @@
   <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +679,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>8</v>
       </c>
@@ -1073,13 +1073,16 @@
       <c r="D129" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E12" xr:uid="{CBE11172-5A0E-4C64-9E83-5BA6D14512AC}">
+  <autoFilter ref="A1:E15" xr:uid="{CBE11172-5A0E-4C64-9E83-5BA6D14512AC}">
     <filterColumn colId="3">
-      <filters blank="1">
+      <filters>
+        <filter val="CheckNextMessage. Every time receiver receives a message, it checks if the message is closing stream"/>
         <filter val="Not Modeled. This section says a lot about message validation and rules and none of it is modeled"/>
         <filter val="SendingISH"/>
-        <filter val="StartingStreamContent -&gt; SendingMessages_x000a_WaitingStreamToStart -&gt; CheckingForValidStanza -&gt; ReceivingMessages"/>
+        <filter val="StartingStreamContent -&gt; SendingMessages_x000a_WaitingStreamToStart -&gt; CheckingForValidStanza -&gt; ReceivingMessages - CheckNextMessage"/>
         <filter val="Waiting ISH -&gt; SendingRSH"/>
+        <filter val="WaitingCST -&gt; EndOfStream (client_checkMessageContent(from,LastCST))"/>
+        <filter val="WaitingCST -&gt; EndOfStream (t&gt;=timeLimit)"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>